<commit_message>
Script for timestamp normalization of syslog files.  Usage:
correctTimestamp <+/- number of minutes>
</commit_message>
<xml_diff>
--- a/Useful Documents/Calculate Samples and Errors.xlsx
+++ b/Useful Documents/Calculate Samples and Errors.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="20520" windowHeight="14000"/>
+    <workbookView xWindow="10640" yWindow="9120" windowWidth="29420" windowHeight="19600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Size of sample required for level of confidence:</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Acceptible Margin of Error (D):</t>
-  </si>
-  <si>
-    <t>Degree of Confidence (Z):</t>
   </si>
   <si>
     <t>Result Confidence:</t>
@@ -341,7 +338,7 @@
             <a:lstStyle/>
             <a:p>
               <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns="">
+                <m:oMathPara xmlns="" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
                     <m:jc m:val="centerGroup"/>
                   </m:oMathParaPr>
@@ -524,7 +521,7 @@
             <a:lstStyle/>
             <a:p>
               <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns="">
+                <m:oMathPara xmlns="" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
                     <m:jc m:val="centerGroup"/>
                   </m:oMathParaPr>
@@ -1560,12 +1557,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1580,23 +1578,18 @@
         <v>13</v>
       </c>
       <c r="F3" s="4">
-        <v>4190</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="4" spans="2:8">
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1.96</v>
-      </c>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="2:8">
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="3">
-        <v>0.05</v>
+        <v>7.5899999999999995E-2</v>
       </c>
     </row>
     <row r="6" spans="2:8">
@@ -1609,7 +1602,7 @@
     </row>
     <row r="8" spans="2:8">
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="17">
         <v>0.9</v>
@@ -1618,23 +1611,23 @@
         <v>11</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:8">
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9">
         <v>1.645</v>
       </c>
       <c r="G9" s="19">
         <f>D9*D9*(F5*(1-F5)/(F6* F6))</f>
-        <v>321.34046875000001</v>
+        <v>474.49600404937496</v>
       </c>
       <c r="H9" s="20">
         <f>G9/(1+(G9/F3))</f>
-        <v>298.45155190327819</v>
+        <v>470.03540561485545</v>
       </c>
     </row>
     <row r="10" spans="2:8">
@@ -1643,7 +1636,7 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="17">
         <v>0.95</v>
@@ -1653,18 +1646,18 @@
     </row>
     <row r="12" spans="2:8">
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12">
         <v>1.96</v>
       </c>
       <c r="G12" s="19">
         <f>D12*D12*(F5*(1-F5)/(F6* F6))</f>
-        <v>456.18999999999994</v>
+        <v>673.61678075999987</v>
       </c>
       <c r="H12" s="20">
         <f>G12/(1+(G12/F3))</f>
-        <v>411.39860832208751</v>
+        <v>664.66222815159495</v>
       </c>
     </row>
     <row r="13" spans="2:8">
@@ -1673,7 +1666,7 @@
     </row>
     <row r="14" spans="2:8">
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="17">
         <v>0.99</v>
@@ -1683,18 +1676,18 @@
     </row>
     <row r="15" spans="2:8">
       <c r="C15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15">
         <v>2.5750000000000002</v>
       </c>
       <c r="G15" s="19">
         <f>D15*D15*(F5*(1-F5)/(F6* F6))</f>
-        <v>787.38671875000011</v>
+        <v>1162.6666667343752</v>
       </c>
       <c r="H15" s="20">
         <f>G15/(1+(G15/F3))</f>
-        <v>662.8278126621102</v>
+        <v>1136.2451788408571</v>
       </c>
     </row>
     <row r="16" spans="2:8">
@@ -1728,7 +1721,7 @@
         <v>2</v>
       </c>
       <c r="E20" s="1">
-        <v>45</v>
+        <v>500</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1736,7 +1729,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="1">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1748,7 +1741,7 @@
       </c>
       <c r="E22" s="2">
         <f>E21/E20</f>
-        <v>4.4444444444444446E-2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1772,7 +1765,7 @@
       <c r="D25" s="10"/>
       <c r="E25" s="2">
         <f>SQRT((E22)*(1-(E22))/E20)*D9</f>
-        <v>5.0535475594406076E-2</v>
+        <v>2.9426654583897236E-2</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="11"/>
@@ -1785,14 +1778,14 @@
       <c r="D26" s="13"/>
       <c r="E26" s="14">
         <f>E22-E25</f>
-        <v>-6.0910311499616301E-3</v>
+        <v>0.17057334541610278</v>
       </c>
       <c r="F26" s="23" t="s">
         <v>7</v>
       </c>
       <c r="G26" s="15">
         <f>E22+E25</f>
-        <v>9.4979920038850529E-2</v>
+        <v>0.22942665458389724</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1816,7 +1809,7 @@
       <c r="D29" s="10"/>
       <c r="E29" s="2">
         <f>SQRT((E22)*(1-(E22))/E20)*D12</f>
-        <v>6.0212481559292347E-2</v>
+        <v>3.5061545887196705E-2</v>
       </c>
       <c r="F29" s="25"/>
       <c r="G29" s="11"/>
@@ -1829,14 +1822,14 @@
       <c r="D30" s="13"/>
       <c r="E30" s="14">
         <f>E22-E29</f>
-        <v>-1.5768037114847901E-2</v>
+        <v>0.16493845411280331</v>
       </c>
       <c r="F30" s="23" t="s">
         <v>7</v>
       </c>
       <c r="G30" s="15">
         <f>E22+E29</f>
-        <v>0.1046569260037368</v>
+        <v>0.23506154588719672</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1860,7 +1853,7 @@
       <c r="D33" s="10"/>
       <c r="E33" s="2">
         <f>SQRT((E22)*(1-(E22))/E20)*D15</f>
-        <v>7.9105683681213165E-2</v>
+        <v>4.6063000336495671E-2</v>
       </c>
       <c r="F33" s="25"/>
       <c r="G33" s="11"/>
@@ -1873,14 +1866,14 @@
       <c r="D34" s="13"/>
       <c r="E34" s="14">
         <f>E22-E33</f>
-        <v>-3.4661239236768719E-2</v>
+        <v>0.15393699966350433</v>
       </c>
       <c r="F34" s="23" t="s">
         <v>7</v>
       </c>
       <c r="G34" s="15">
         <f>E22+E33</f>
-        <v>0.1235501281256576</v>
+        <v>0.2460630003364957</v>
       </c>
     </row>
   </sheetData>

</xml_diff>